<commit_message>
co and reg update
</commit_message>
<xml_diff>
--- a/zinfo/CosAndRegistrars.xlsx
+++ b/zinfo/CosAndRegistrars.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+  <si>
+    <t xml:space="preserve">Co Type</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Co Ticker</t>
+  </si>
+  <si>
     <t xml:space="preserve">Address 1</t>
   </si>
   <si>
@@ -46,6 +52,30 @@
     <t xml:space="preserve">email</t>
   </si>
   <si>
+    <t xml:space="preserve">Manages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al-noor Sugar Mill (Pvt) Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALNRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96-A, Sindhi Muslim Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karachi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3450161-63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrar</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDC Share Registrar Services Limited – Head Office – CDC House</t>
   </si>
   <si>
@@ -55,9 +85,6 @@
     <t xml:space="preserve">Main Shahra-e-Faisal</t>
   </si>
   <si>
-    <t xml:space="preserve">Karachi</t>
-  </si>
-  <si>
     <t xml:space="preserve">(92) 0800-23275</t>
   </si>
   <si>
@@ -85,32 +112,28 @@
     <t xml:space="preserve">M 13, Progressive Plaza, Plot No 5 – CL – 10</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Civil Lines Quarter, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Near P.I.D.C, Beaumont Road</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Al-noor Sugar Mill (Pvt) Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96-A, Sindhi Muslim Society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3450161-63</t>
+    <t xml:space="preserve">Civil Lines Quarter, Near P.I.D.C, Beaumont Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sitara Chemical Industries Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THK Associates (Pvt.) Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot No. 32-C, Jami Commercial Street 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.H.A. Phase VII</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9221 5310191-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sfc@thk.com.pk</t>
   </si>
 </sst>
 </file>
@@ -151,8 +174,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,7 +222,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -207,6 +232,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,6 +252,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -337,26 +383,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="55.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="41.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -380,88 +428,153 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>74400</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>74400</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>75530</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <v>74400</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>75530</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>74400</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
+      <c r="G7" s="1" t="n">
+        <v>75500</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="info@cdcsrl.com"/>
-    <hyperlink ref="H3" r:id="rId2" display="info@cdcsrl.com"/>
+    <hyperlink ref="J3" r:id="rId1" display="info@cdcsrl.com"/>
+    <hyperlink ref="J4" r:id="rId2" display="info@cdcsrl.com"/>
+    <hyperlink ref="J7" r:id="rId3" display="sfc@thk.com.pk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
haleon, inquiry and address updated
</commit_message>
<xml_diff>
--- a/zinfo/CosAndRegistrars.xlsx
+++ b/zinfo/CosAndRegistrars.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -146,6 +146,45 @@
   </si>
   <si>
     <t xml:space="preserve">(92-42) 36362061-66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haleon Pakistan Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HALEON</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">11-A, 11</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Floor, Sky Tower (East Wing)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolmen City, HC-3, Block 4, Scheme-5, Clifton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">021 111 425 366</t>
   </si>
   <si>
     <t xml:space="preserve">M/s. C &amp; K Management Associates (Pvt) Limited</t>
@@ -288,7 +327,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -316,6 +355,17 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -367,12 +417,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,6 +431,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,6 +455,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -515,14 +586,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A:A"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,56 +792,62 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E6" s="2" t="n">
+        <v>403</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="G6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>75530</v>
+        <v>75600</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G7" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="H7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="2" t="n">
-        <v>82</v>
+        <v>25</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>75530</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>20</v>
@@ -784,163 +861,189 @@
       <c r="E8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>75800</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="N8" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="O8" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P8" s="2" t="n">
-        <v>2872</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="T8" s="2" t="n">
-        <v>154</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="I9" s="2" t="n">
+        <v>75800</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="N9" s="2" t="n">
-        <v>1768</v>
+        <v>21</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>248</v>
-      </c>
-      <c r="P9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>2872</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="R9" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T9" s="2" t="n">
-        <v>248</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>68</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>1768</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>248</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <v>248</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>75500</v>
-      </c>
-      <c r="J11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>567</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>76</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="2" t="n">
+        <v>75500</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>567</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="2" t="n">
         <v>45530</v>
       </c>
-      <c r="N12" s="2" t="n">
+      <c r="N13" s="2" t="n">
         <v>55</v>
       </c>
     </row>
@@ -948,7 +1051,7 @@
   <hyperlinks>
     <hyperlink ref="L4" r:id="rId1" display="info@cdcsrl.com"/>
     <hyperlink ref="L5" r:id="rId2" display="info@cdcsrl.com"/>
-    <hyperlink ref="L11" r:id="rId3" display="sfc@thk.com.pk"/>
+    <hyperlink ref="L12" r:id="rId3" display="sfc@thk.com.pk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>